<commit_message>
[FileMS] Update Import Logic
</commit_message>
<xml_diff>
--- a/Microservices/FilesMicroservice/Files.Api/wwwroot/templates/ProductTemplate.xlsx
+++ b/Microservices/FilesMicroservice/Files.Api/wwwroot/templates/ProductTemplate.xlsx
@@ -12,21 +12,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>ID</t>
+    <t>ProductNumber</t>
   </si>
   <si>
     <t>ProductName</t>
   </si>
   <si>
-    <t>ProductCode</t>
+    <t>QtyPerPackage</t>
   </si>
   <si>
-    <t>ProductNumber</t>
-  </si>
-  <si>
-    <t>Quantity</t>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
@@ -34,21 +31,31 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00" tint="0"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -56,12 +63,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -72,30 +93,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="30" customWidth="1" style="1"/>
+    <col min="2" max="2" width="30" customWidth="1" style="1"/>
+    <col min="3" max="3" width="30" customWidth="1" style="1"/>
+    <col min="4" max="4" width="30" customWidth="1" style="1"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[Angular][FileMS] Update Import Feature
</commit_message>
<xml_diff>
--- a/Microservices/FilesMicroservice/Files.Api/wwwroot/templates/ProductTemplate.xlsx
+++ b/Microservices/FilesMicroservice/Files.Api/wwwroot/templates/ProductTemplate.xlsx
@@ -64,10 +64,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -76,7 +76,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" borderId="1" applyBorder="1" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>

</xml_diff>